<commit_message>
Prepping for publication - Mar 30, 2022
</commit_message>
<xml_diff>
--- a/data/ROV/ROVPres_Abs_All.xlsx
+++ b/data/ROV/ROVPres_Abs_All.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samstarko/Dropbox/Barkley Sound Kelp Monitoring/Subtidal Canopy Kelps/SubtidalKelps2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samstarko/Dropbox/R_projects/SubtidalKelps3/data/ROV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E609DD5E-CFC2-3144-B7C7-083EC5D7D5D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBAF1E3-43C1-8841-BC55-7AC98B53E6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="1420" windowWidth="27640" windowHeight="16060" xr2:uid="{2E48FB2B-F6FA-C34F-B3AB-540EC429DF08}"/>
+    <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="16060" xr2:uid="{2E48FB2B-F6FA-C34F-B3AB-540EC429DF08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
   <si>
     <t>rov_site_id</t>
   </si>
@@ -93,9 +93,6 @@
     <t xml:space="preserve">, </t>
   </si>
   <si>
-    <t>Coordinates fixed</t>
-  </si>
-  <si>
     <t>Nereo</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>27B</t>
   </si>
   <si>
-    <t>Note to throw this one out in main analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve">haphazard </t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>Line connecting KB4 sites</t>
+  </si>
+  <si>
+    <t>Kelp</t>
+  </si>
+  <si>
+    <t>Note to throw this data point should not be used due to replicate with "27"</t>
   </si>
 </sst>
 </file>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FFDA07-F136-854B-856A-4C1BD5856A17}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,7 +573,7 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,15 +590,18 @@
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1">
         <v>48.8436333</v>
@@ -612,8 +615,12 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="b">
+        <f>OR(E2=1,F2=1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>23</v>
       </c>
@@ -632,11 +639,12 @@
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="b">
+        <f t="shared" ref="G3:G66" si="0">OR(E3=1,F3=1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -655,11 +663,12 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>7</v>
       </c>
@@ -678,9 +687,13 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>11</v>
       </c>
@@ -699,8 +712,12 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -719,8 +736,12 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>9</v>
       </c>
@@ -739,11 +760,15 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>19</v>
       </c>
@@ -762,8 +787,12 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -782,8 +811,12 @@
       <c r="F10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -802,8 +835,12 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -822,8 +859,12 @@
       <c r="F12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -842,8 +883,12 @@
       <c r="F13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -862,8 +907,12 @@
       <c r="F14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>25</v>
       </c>
@@ -882,8 +931,12 @@
       <c r="F15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>22</v>
       </c>
@@ -900,6 +953,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="b">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -922,6 +979,10 @@
       <c r="F17" s="1">
         <v>0</v>
       </c>
+      <c r="G17" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -942,6 +1003,10 @@
       <c r="F18" s="1">
         <v>0</v>
       </c>
+      <c r="G18" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -962,8 +1027,9 @@
       <c r="F19" s="1">
         <v>0</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>19</v>
+      <c r="G19" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -985,6 +1051,10 @@
       <c r="F20" s="1">
         <v>0</v>
       </c>
+      <c r="G20" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1005,6 +1075,10 @@
       <c r="F21" s="1">
         <v>0</v>
       </c>
+      <c r="G21" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1025,6 +1099,10 @@
       <c r="F22" s="1">
         <v>0</v>
       </c>
+      <c r="G22" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1045,6 +1123,10 @@
       <c r="F23" s="1">
         <v>0</v>
       </c>
+      <c r="G23" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1065,6 +1147,10 @@
       <c r="F24" s="1">
         <v>0</v>
       </c>
+      <c r="G24" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1085,6 +1171,10 @@
       <c r="F25" s="1">
         <v>0</v>
       </c>
+      <c r="G25" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1105,6 +1195,10 @@
       <c r="F26" s="1">
         <v>0</v>
       </c>
+      <c r="G26" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1125,6 +1219,10 @@
       <c r="F27" s="1">
         <v>0</v>
       </c>
+      <c r="G27" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1145,6 +1243,10 @@
       <c r="F28" s="1">
         <v>0</v>
       </c>
+      <c r="G28" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1165,10 +1267,14 @@
       <c r="F29" s="1">
         <v>0</v>
       </c>
+      <c r="G29" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
@@ -1185,10 +1291,14 @@
       <c r="F30" s="1">
         <v>0</v>
       </c>
+      <c r="G30" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
@@ -1205,10 +1315,14 @@
       <c r="F31" s="1">
         <v>0</v>
       </c>
+      <c r="G31" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
@@ -1225,10 +1339,14 @@
       <c r="F32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1">
         <v>48.865682999999997</v>
@@ -1242,10 +1360,14 @@
       <c r="F33" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>14</v>
@@ -1262,8 +1384,12 @@
       <c r="F34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
@@ -1279,8 +1405,12 @@
       <c r="F35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -1299,8 +1429,12 @@
       <c r="F36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>29</v>
       </c>
@@ -1319,8 +1453,12 @@
       <c r="F37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>28</v>
       </c>
@@ -1339,8 +1477,12 @@
       <c r="F38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>30</v>
       </c>
@@ -1359,10 +1501,14 @@
       <c r="F39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
@@ -1379,11 +1525,15 @@
       <c r="F40" s="1">
         <v>0</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>32</v>
       </c>
@@ -1402,8 +1552,12 @@
       <c r="F41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>34</v>
       </c>
@@ -1422,8 +1576,12 @@
       <c r="F42" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>35</v>
       </c>
@@ -1442,11 +1600,12 @@
       <c r="F43" s="1">
         <v>0</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>36</v>
       </c>
@@ -1465,10 +1624,14 @@
       <c r="F44" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>13</v>
@@ -1485,10 +1648,14 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>13</v>
@@ -1505,10 +1672,14 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>13</v>
@@ -1525,10 +1696,14 @@
       <c r="F47" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>13</v>
@@ -1545,8 +1720,12 @@
       <c r="F48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>27</v>
       </c>
@@ -1565,8 +1744,12 @@
       <c r="F49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -1585,8 +1768,12 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
@@ -1605,8 +1792,12 @@
       <c r="F51" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>6</v>
       </c>
@@ -1625,8 +1816,12 @@
       <c r="F52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
@@ -1645,8 +1840,12 @@
       <c r="F53" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
@@ -1665,8 +1864,12 @@
       <c r="F54" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
@@ -1685,8 +1888,12 @@
       <c r="F55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>10</v>
       </c>
@@ -1705,13 +1912,17 @@
       <c r="F56" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C57" s="3">
         <v>48.864032999999999</v>
@@ -1725,13 +1936,17 @@
       <c r="F57" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C58" s="3">
         <v>48.859050000000003</v>
@@ -1745,13 +1960,17 @@
       <c r="F58" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C59" s="3">
         <v>48.853450000000002</v>
@@ -1765,13 +1984,17 @@
       <c r="F59" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C60" s="3">
         <v>48.854044999999999</v>
@@ -1785,13 +2008,17 @@
       <c r="F60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C61" s="3">
         <v>48.839799999999997</v>
@@ -1805,13 +2032,17 @@
       <c r="F61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C62" s="3">
         <v>48.838957999999998</v>
@@ -1825,13 +2056,17 @@
       <c r="F62" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C63" s="4">
         <v>48.853069439999999</v>
@@ -1845,13 +2080,17 @@
       <c r="F63" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C64" s="4">
         <v>48.871119999999998</v>
@@ -1865,13 +2104,17 @@
       <c r="F64" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G64" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C65" s="5">
         <v>48.879809999999999</v>
@@ -1885,16 +2128,20 @@
       <c r="F65" s="1">
         <v>0</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G65" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="B66" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C66" s="5">
         <v>48.881509999999999</v>
@@ -1908,13 +2155,17 @@
       <c r="F66" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C67" s="1">
         <v>48.871299999999998</v>
@@ -1928,16 +2179,20 @@
       <c r="F67" s="1">
         <v>0</v>
       </c>
-      <c r="G67" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G67" s="1" t="b">
+        <f t="shared" ref="G67:G68" si="1">OR(E67=1,F67=1)</f>
+        <v>0</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C68" s="1">
         <v>48.873454000000002</v>
@@ -1949,6 +2204,10 @@
         <v>0</v>
       </c>
       <c r="F68" s="1">
+        <v>0</v>
+      </c>
+      <c r="G68" s="1" t="b">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>